<commit_message>
refactor: 4 new fields
</commit_message>
<xml_diff>
--- a/helpers/templates/deliveryArticles/rdn1.xlsx
+++ b/helpers/templates/deliveryArticles/rdn1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="177">
   <si>
     <t>ParentKey</t>
   </si>
@@ -331,6 +331,15 @@
   </si>
   <si>
     <t>ShipToDescription</t>
+  </si>
+  <si>
+    <t>WhsCode</t>
+  </si>
+  <si>
+    <t>U_L_P_Origen</t>
+  </si>
+  <si>
+    <t>U_L_P_Destino</t>
   </si>
   <si>
     <t>U_MontoUSD</t>
@@ -356,9 +365,6 @@
   </si>
   <si>
     <t>DiscPrcnt</t>
-  </si>
-  <si>
-    <t>WhsCode</t>
   </si>
   <si>
     <t>SlpCode</t>
@@ -630,7 +636,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -645,6 +651,9 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -952,7 +961,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:DE2"/>
+  <dimension ref="A1:DH2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -1063,13 +1072,16 @@
     <col min="103" max="103" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="104" max="104" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="105" max="105" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="106" max="106" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="107" max="107" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="108" max="108" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="109" max="109" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="106" max="106" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="107" max="107" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="108" max="108" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="109" max="109" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="110" max="110" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="111" max="111" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="112" max="112" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1394,13 +1406,22 @@
       <c r="DD1" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="DE1" s="3" t="s">
+      <c r="DE1" s="4" t="s">
         <v>108</v>
       </c>
+      <c r="DF1" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="DG1" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="DH1" s="3" t="s">
+        <v>111</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="5" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>1</v>
@@ -1409,7 +1430,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>4</v>
@@ -1421,7 +1442,7 @@
         <v>6</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>8</v>
@@ -1430,7 +1451,7 @@
         <v>9</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>11</v>
@@ -1439,34 +1460,34 @@
         <v>12</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="Q2" s="5" t="s">
         <v>16</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="X2" s="5" t="s">
         <v>23</v>
@@ -1475,37 +1496,37 @@
         <v>24</v>
       </c>
       <c r="Z2" s="5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="AA2" s="5" t="s">
         <v>26</v>
       </c>
       <c r="AB2" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="AC2" s="5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="AD2" s="5" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="AE2" s="5" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="AF2" s="5" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="AG2" s="5" t="s">
         <v>32</v>
       </c>
       <c r="AH2" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="AI2" s="5" t="s">
         <v>34</v>
       </c>
       <c r="AJ2" s="5" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="AK2" s="5" t="s">
         <v>36</v>
@@ -1532,19 +1553,19 @@
         <v>43</v>
       </c>
       <c r="AS2" s="5" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AT2" s="5" t="s">
         <v>45</v>
       </c>
       <c r="AU2" s="5" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="AV2" s="5" t="s">
         <v>47</v>
       </c>
       <c r="AW2" s="5" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="AX2" s="5" t="s">
         <v>49</v>
@@ -1556,52 +1577,52 @@
         <v>51</v>
       </c>
       <c r="BA2" s="5" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="BB2" s="5" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="BC2" s="5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="BD2" s="5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="BE2" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="BF2" s="5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="BG2" s="5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="BH2" s="5" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="BI2" s="5" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="BJ2" s="5" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="BK2" s="5" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="BL2" s="5" t="s">
         <v>63</v>
       </c>
       <c r="BM2" s="5" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="BN2" s="5" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="BO2" s="5" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="BP2" s="5" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="BQ2" s="5" t="s">
         <v>68</v>
@@ -1610,16 +1631,16 @@
         <v>69</v>
       </c>
       <c r="BS2" s="5" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="BT2" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="BU2" s="5" t="s">
         <v>72</v>
       </c>
       <c r="BV2" s="5" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="BW2" s="5" t="s">
         <v>74</v>
@@ -1634,7 +1655,7 @@
         <v>77</v>
       </c>
       <c r="CA2" s="5" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="CB2" s="5" t="s">
         <v>79</v>
@@ -1643,76 +1664,76 @@
         <v>80</v>
       </c>
       <c r="CD2" s="5" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="CE2" s="5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="CF2" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="CG2" s="5" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="CH2" s="5" t="s">
         <v>85</v>
       </c>
       <c r="CI2" s="5" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="CJ2" s="5" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="CK2" s="5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="CL2" s="5" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="CM2" s="5" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="CN2" s="5" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="CO2" s="5" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="CP2" s="5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="CQ2" s="5" t="s">
         <v>94</v>
       </c>
       <c r="CR2" s="5" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="CS2" s="5" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="CT2" s="5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="CU2" s="5" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="CV2" s="5" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="CW2" s="5" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="CX2" s="5" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="CY2" s="5" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="CZ2" s="5" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="DA2" s="5" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="DB2" s="4" t="s">
         <v>105</v>
@@ -1723,8 +1744,17 @@
       <c r="DD2" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="DE2" s="5" t="s">
-        <v>174</v>
+      <c r="DE2" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="DF2" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="DG2" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="DH2" s="5" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>